<commit_message>
Registration Test Data 1
</commit_message>
<xml_diff>
--- a/src/main/java/testData/LoginDetails.xlsx
+++ b/src/main/java/testData/LoginDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingis/eclipse-workspace/CalendarAppCopy/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2B5F52-85A1-3F4A-98CA-A9F1B7C378F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EAC7AA-A88E-C041-A16E-D8E174699AA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{8FEFF26B-84DC-3F4E-92B7-5144F87B859F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{8FEFF26B-84DC-3F4E-92B7-5144F87B859F}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -67,9 +67,6 @@
     <t>akhilbingi@gmail.com</t>
   </si>
   <si>
-    <t>akhilbingi32</t>
-  </si>
-  <si>
     <t>Matrix@321456</t>
   </si>
   <si>
@@ -91,18 +88,9 @@
     <t>akhilbingi64@gmail.com</t>
   </si>
   <si>
-    <t>akhilbingi321</t>
-  </si>
-  <si>
     <t>""</t>
   </si>
   <si>
-    <t>akhilbingi3212</t>
-  </si>
-  <si>
-    <t>akhilhdiw</t>
-  </si>
-  <si>
     <t>aka</t>
   </si>
   <si>
@@ -112,7 +100,28 @@
     <t>akabc</t>
   </si>
   <si>
-    <t>akhilhdingi</t>
+    <t>akhilbingi3213</t>
+  </si>
+  <si>
+    <t>akhilbingi6423444</t>
+  </si>
+  <si>
+    <t>akhilbingi324455</t>
+  </si>
+  <si>
+    <t>akhilbingi321566</t>
+  </si>
+  <si>
+    <t>akhilbingi3212777</t>
+  </si>
+  <si>
+    <t>nffmf88</t>
+  </si>
+  <si>
+    <t>akhilhdiw599</t>
+  </si>
+  <si>
+    <t>akhilhdingi900</t>
   </si>
 </sst>
 </file>
@@ -545,14 +554,14 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -579,13 +588,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -593,16 +602,16 @@
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
@@ -610,16 +619,16 @@
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
@@ -630,13 +639,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
@@ -647,13 +656,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
@@ -664,11 +673,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
@@ -679,13 +690,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
@@ -693,22 +704,25 @@
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="akhilbingi6423@gmail.com" xr:uid="{FF364A20-4455-7048-9DF5-DE60DB4F651A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Registration Page test Data 2
</commit_message>
<xml_diff>
--- a/src/main/java/testData/LoginDetails.xlsx
+++ b/src/main/java/testData/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingis/eclipse-workspace/CalendarAppCopy/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EAC7AA-A88E-C041-A16E-D8E174699AA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC86D20-2581-EE4A-8630-67C8ADC9FA2E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{8FEFF26B-84DC-3F4E-92B7-5144F87B859F}"/>
   </bookViews>
@@ -100,28 +100,28 @@
     <t>akabc</t>
   </si>
   <si>
-    <t>akhilbingi3213</t>
-  </si>
-  <si>
-    <t>akhilbingi6423444</t>
-  </si>
-  <si>
-    <t>akhilbingi324455</t>
-  </si>
-  <si>
-    <t>akhilbingi321566</t>
-  </si>
-  <si>
-    <t>akhilbingi3212777</t>
-  </si>
-  <si>
-    <t>nffmf88</t>
-  </si>
-  <si>
-    <t>akhilhdiw599</t>
-  </si>
-  <si>
-    <t>akhilhdingi900</t>
+    <t>akhilbingi32131</t>
+  </si>
+  <si>
+    <t>akhilbingi64234442</t>
+  </si>
+  <si>
+    <t>akhilbingi3244553</t>
+  </si>
+  <si>
+    <t>akhilbingi3215664</t>
+  </si>
+  <si>
+    <t>akhilbingi32127775</t>
+  </si>
+  <si>
+    <t>nffmf886</t>
+  </si>
+  <si>
+    <t>akhilhdiw5997</t>
+  </si>
+  <si>
+    <t>akhilhdingi9008</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -703,8 +703,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
+      <c r="A9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Registration Page Test Data 3
</commit_message>
<xml_diff>
--- a/src/main/java/testData/LoginDetails.xlsx
+++ b/src/main/java/testData/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingis/eclipse-workspace/CalendarAppCopy/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC86D20-2581-EE4A-8630-67C8ADC9FA2E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA08327-2C2D-014B-B9F6-DF12ADD09E00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{8FEFF26B-84DC-3F4E-92B7-5144F87B859F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Username</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>akhilhdingi9008</t>
+  </si>
+  <si>
+    <t>ak@gmail.com</t>
+  </si>
+  <si>
+    <t>bingi18</t>
+  </si>
+  <si>
+    <t>RoyalEnfield</t>
   </si>
 </sst>
 </file>
@@ -551,10 +560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF42965B-7184-1B4C-B5EF-9BB1D84BE67B}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,9 +728,27 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="akhilbingi6423@gmail.com" xr:uid="{FF364A20-4455-7048-9DF5-DE60DB4F651A}"/>
+    <hyperlink ref="A10" r:id="rId2" xr:uid="{78D812E6-FA85-2145-A7A1-D877B7D3C668}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Automatically Build project when there is new build
</commit_message>
<xml_diff>
--- a/src/main/java/testData/LoginDetails.xlsx
+++ b/src/main/java/testData/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingis/eclipse-workspace/CalendarAppCopy/src/main/java/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611D4C04-0AD2-584D-920D-3DF53DE20D5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E65B60-1563-4A41-AA37-AC903E793399}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{8FEFF26B-84DC-3F4E-92B7-5144F87B859F}"/>
   </bookViews>
@@ -100,37 +100,37 @@
     <t>akabc</t>
   </si>
   <si>
-    <t>akhilbingi32131</t>
-  </si>
-  <si>
-    <t>akhilbingi64234442</t>
-  </si>
-  <si>
-    <t>akhilbingi3244553</t>
-  </si>
-  <si>
-    <t>akhilbingi3215664</t>
-  </si>
-  <si>
-    <t>akhilbingi32127775</t>
-  </si>
-  <si>
-    <t>nffmf886</t>
-  </si>
-  <si>
-    <t>akhilhdiw5997</t>
-  </si>
-  <si>
-    <t>akhilhdingi9008</t>
-  </si>
-  <si>
     <t>ak@gmail.com</t>
   </si>
   <si>
     <t>bingi18</t>
   </si>
   <si>
-    <t>RoyalEnfield</t>
+    <t>akhilbingi321312</t>
+  </si>
+  <si>
+    <t>akhilbingi642344423</t>
+  </si>
+  <si>
+    <t>akhilbingi32445534</t>
+  </si>
+  <si>
+    <t>akhilbingi32156645</t>
+  </si>
+  <si>
+    <t>akhilbingi321277756</t>
+  </si>
+  <si>
+    <t>nffmf8867</t>
+  </si>
+  <si>
+    <t>akhilhdiw59978</t>
+  </si>
+  <si>
+    <t>akhilhdingi90089</t>
+  </si>
+  <si>
+    <t>RoyalEnfield1</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,7 +600,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -617,7 +617,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
@@ -634,7 +634,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -651,7 +651,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -668,7 +668,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -685,7 +685,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -702,7 +702,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>18</v>
@@ -719,7 +719,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -730,10 +730,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>

</xml_diff>